<commit_message>
Update D3a_Mapa prava i usluga_BOS.xlsx
</commit_message>
<xml_diff>
--- a/D3a_Mapa prava i usluga_BOS.xlsx
+++ b/D3a_Mapa prava i usluga_BOS.xlsx
@@ -8,35 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anes-PC\Github\amra-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAF20582-E8A9-486C-B935-8EC2C178D0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B07A1D-37C1-42D2-97D5-F1800B8EA1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="975" firstSheet="8" activeTab="11" xr2:uid="{6DCFD875-645F-4B85-AAFB-14BA6F769E6A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="975" firstSheet="9" activeTab="11" xr2:uid="{6DCFD875-645F-4B85-AAFB-14BA6F769E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter" sheetId="14" state="hidden" r:id="rId1"/>
     <sheet name="Pivot" sheetId="18" state="hidden" r:id="rId2"/>
     <sheet name="All (2)" sheetId="17" state="hidden" r:id="rId3"/>
-    <sheet name="HOME" sheetId="6" r:id="rId4"/>
-    <sheet name="Dijagnoza" sheetId="24" r:id="rId5"/>
-    <sheet name="Predskolska" sheetId="8" r:id="rId6"/>
-    <sheet name="Skolska" sheetId="9" r:id="rId7"/>
-    <sheet name="Radni vijek" sheetId="11" r:id="rId8"/>
-    <sheet name="Treca dob" sheetId="12" r:id="rId9"/>
-    <sheet name="Dashboard" sheetId="3" state="hidden" r:id="rId10"/>
-    <sheet name="Neinstitucionalizirana prava" sheetId="13" r:id="rId11"/>
-    <sheet name="Administrativni postupci" sheetId="1" r:id="rId12"/>
-    <sheet name="Diskrecione usluge" sheetId="5" r:id="rId13"/>
-    <sheet name="All" sheetId="15" state="hidden" r:id="rId14"/>
-    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="25" r:id="rId4"/>
+    <sheet name="HOME" sheetId="6" r:id="rId5"/>
+    <sheet name="Dijagnoza" sheetId="24" r:id="rId6"/>
+    <sheet name="Predskolska" sheetId="8" r:id="rId7"/>
+    <sheet name="Skolska" sheetId="9" r:id="rId8"/>
+    <sheet name="Radni vijek" sheetId="11" r:id="rId9"/>
+    <sheet name="Treca dob" sheetId="12" r:id="rId10"/>
+    <sheet name="Dashboard" sheetId="3" state="hidden" r:id="rId11"/>
+    <sheet name="Neinstitucionalizirana prava" sheetId="13" r:id="rId12"/>
+    <sheet name="Administrativni postupci" sheetId="1" r:id="rId13"/>
+    <sheet name="Diskrecione usluge" sheetId="5" r:id="rId14"/>
+    <sheet name="All" sheetId="15" state="hidden" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId16"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId17"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Administrativni postupci'!$A$1:$Q$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">All!$A$1:$P$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Administrativni postupci'!$A$1:$Q$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">All!$A$1:$P$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'All (2)'!$A$1:$P$175</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Diskrecione usluge'!$O$1:$O$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Diskrecione usluge'!$O$1:$O$28</definedName>
+    <definedName name="All" localSheetId="3">[1]All!$B$35:$P$54</definedName>
     <definedName name="All">All!$B$35:$P$54</definedName>
+    <definedName name="Ambulanta__Sve_na_jednom_mjestu__za_djecu_i_osobe_s_poteškoćama_u_razvoju" localSheetId="3">[1]Sheet2!$E$2:INDEX([1]Sheet2!$E:$E,COUNTA([1]Sheet2!$E:$E))</definedName>
     <definedName name="Ambulanta__Sve_na_jednom_mjestu__za_djecu_i_osobe_s_poteškoćama_u_razvoju">Sheet2!$E$2:INDEX(Sheet2!$E:$E,COUNTA(Sheet2!$E:$E))</definedName>
     <definedName name="dob">Sheet2!$D$2:$D$8</definedName>
+    <definedName name="N" localSheetId="3">OFFSET([1]Sheet2!$E$2, 0, 0, COUNTA([1]Sheet2!$E:$E), 1)</definedName>
     <definedName name="N">OFFSET(Sheet2!$E$2, 0, 0, COUNTA(Sheet2!$E:$E), 1)</definedName>
     <definedName name="Novorodjence">Sheet2!$E$2:$E$32</definedName>
     <definedName name="Postupci">'Administrativni postupci'!$B$2:$B$45</definedName>
@@ -47,14 +54,14 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId17"/>
-        <x14:slicerCache r:id="rId18"/>
         <x14:slicerCache r:id="rId19"/>
+        <x14:slicerCache r:id="rId20"/>
+        <x14:slicerCache r:id="rId21"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -357,7 +364,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="564">
   <si>
     <t>Životna dob</t>
   </si>
@@ -2960,6 +2967,12 @@
       </rPr>
       <t>Ova mapa na naglašava specifičan skup prava koja su eksluzivno vezana za ratni invaliditet i koja su priznata isključivo osobama sa statusam RVI ili članovima njihovih porodica.</t>
     </r>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
   </si>
 </sst>
 </file>
@@ -3334,7 +3347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -3521,12 +3534,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3925,11 +3973,14 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3937,17 +3988,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3958,15 +4009,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="59">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4016,6 +4079,92 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF374151"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF374151"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6594,6 +6743,1003 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Filter"/>
+      <sheetName val="Pivot"/>
+      <sheetName val="All (2)"/>
+      <sheetName val="HOME"/>
+      <sheetName val="Dijagnoza"/>
+      <sheetName val="1"/>
+      <sheetName val="2"/>
+      <sheetName val="3"/>
+      <sheetName val="4"/>
+      <sheetName val="5"/>
+      <sheetName val="Dashboard"/>
+      <sheetName val="Neinstitucionalizirana prava"/>
+      <sheetName val="Administrativni postupci"/>
+      <sheetName val="Diskrecione usluge"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="RASPORED ZA INFOGRAFIKU"/>
+      <sheetName val="INFOGRAF"/>
+      <sheetName val="All"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Adresa</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Lat</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Lon</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Kranjčevićeva 12, Sarajevo</v>
+          </cell>
+          <cell r="B2">
+            <v>43.858553000000001</v>
+          </cell>
+          <cell r="C2">
+            <v>18.402099609375</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v xml:space="preserve"> Reisa Džemaludina Čauševića 1, 71000 Sarajevo     </v>
+          </cell>
+          <cell r="B3">
+            <v>43.857349450000001</v>
+          </cell>
+          <cell r="C3">
+            <v>18.413135847170199</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Butmirska cesta 12, prvi sprat</v>
+          </cell>
+          <cell r="B4">
+            <v>43.829455600000003</v>
+          </cell>
+          <cell r="C4">
+            <v>18.310951865680199</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Bulevar Meše Selimovića 12</v>
+          </cell>
+          <cell r="B5">
+            <v>43.847950949999998</v>
+          </cell>
+          <cell r="C5">
+            <v>18.3536972495775</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Zmaja od Bosne 88</v>
+          </cell>
+          <cell r="B6">
+            <v>43.852587649999997</v>
+          </cell>
+          <cell r="C6">
+            <v>18.3816443990954</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Ložionička 2</v>
+          </cell>
+          <cell r="B7">
+            <v>43.85633</v>
+          </cell>
+          <cell r="C7">
+            <v>18.384492399999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v xml:space="preserve">Reisa Džemaludina Čauševića 1, 71000 Sarajevo     </v>
+          </cell>
+          <cell r="B8">
+            <v>43.857349450000001</v>
+          </cell>
+          <cell r="C8">
+            <v>18.413135847170199</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>Bolnička 4, Sarajevo</v>
+          </cell>
+          <cell r="B9">
+            <v>43.8671705</v>
+          </cell>
+          <cell r="C9">
+            <v>18.413270799999999</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Aleja Bosne Srebrene 7
+71000 Sarajevo</v>
+          </cell>
+          <cell r="B10">
+            <v>43.833867749999897</v>
+          </cell>
+          <cell r="C10">
+            <v>18.3318392646853</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Primjer Općine Centar</v>
+          </cell>
+          <cell r="B11">
+            <v>43.899231149999999</v>
+          </cell>
+          <cell r="C11">
+            <v>18.4151610950864</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>La Benevolencija 16</v>
+          </cell>
+          <cell r="B12">
+            <v>43.857481149999998</v>
+          </cell>
+          <cell r="C12">
+            <v>18.416157265859901</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Zmaja od Bosne 55, 71000 Sarajevo, Bosna i Hercegovina</v>
+          </cell>
+          <cell r="B13">
+            <v>43.851796999999998</v>
+          </cell>
+          <cell r="C13">
+            <v>18.3827719453942</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>Reisa Džemaludina Čauševića 1, Sarajevo</v>
+          </cell>
+          <cell r="B14">
+            <v>43.857349450000001</v>
+          </cell>
+          <cell r="C14">
+            <v>18.413135847170199</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Mis Irbina 1, 71000 Sarajevo, BiH</v>
+          </cell>
+          <cell r="B15">
+            <v>43.857201400000001</v>
+          </cell>
+          <cell r="C15">
+            <v>18.413743400000001</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Ložionička 2, 71000 Sarajevo, Bosna i Hercegovina</v>
+          </cell>
+          <cell r="B16">
+            <v>43.85633</v>
+          </cell>
+          <cell r="C16">
+            <v>18.384492399999999</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Bulevar Meše Selimovića 97
+71000 Sarajevo, BiH</v>
+          </cell>
+          <cell r="B17">
+            <v>43.84666275</v>
+          </cell>
+          <cell r="C17">
+            <v>18.354620012764201</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Gatačka 80, Sarajevo</v>
+          </cell>
+          <cell r="B18">
+            <v>43.843953499999998</v>
+          </cell>
+          <cell r="C18">
+            <v>18.358142300000001</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Vilsonovo šetalište 10</v>
+          </cell>
+          <cell r="B19">
+            <v>43.85358815</v>
+          </cell>
+          <cell r="C19">
+            <v>18.394800338932299</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Bjelave 52, 71000 Sarajevo, Bosna i Hercegovina</v>
+          </cell>
+          <cell r="B20">
+            <v>43.856848849999999</v>
+          </cell>
+          <cell r="C20">
+            <v>18.384989102369499</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17">
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>Ambulanta "Sve na jednom mjestu" za djecu i osobe s poteškoćama u razvoju</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>Dodatna ambulanta nije namijenjena za prehlade, upale grla i sl. Nego, ukoliko dijete ili osoba sa teškoćama u razvoju treba istovremeno preglede, odnosno nalaze, kao što su vađenje krvi, EKG, RTG pluća, pedijatrijski pregled ili mišljenje anesteziologa.</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="E35" t="str">
+            <v>Zdravstvena zaštita</v>
+          </cell>
+          <cell r="F35" t="str">
+            <v>Opća bolnica "Prim.dr. Abdulah Nakaš"</v>
+          </cell>
+          <cell r="G35" t="str">
+            <v>Kranjčevićeva 12, Sarajevo</v>
+          </cell>
+          <cell r="I35">
+            <v>38733285261</v>
+          </cell>
+          <cell r="L35" t="str">
+            <v>Naručivanje u ambulanti.</v>
+          </cell>
+          <cell r="P35" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>Asistent u nastavi</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v>Asistenti u nastavi se uvode sa ciljem da, u skladu sa potrebama djece, pruže pomoć i podršku inkluzivnom obrazovanju. Predstavljaju pomoć odgajatelju/nastavniku i stručnim saradnjicima u cilju unapređenja njihovog rada sa dijecom. IPP definira potrebu za asistentima u nastavi. Obuku, akreditaciju asistenata i nadzor nad radom asistenata vrši Prosvjetno-pedagoški zavod, u skladu sa propisom koji donosi ministar.</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>Školska dob</v>
+          </cell>
+          <cell r="E36" t="str">
+            <v>Obrazovanje</v>
+          </cell>
+          <cell r="F36" t="str">
+            <v>Ministarstvo odgoja i obrazovanja</v>
+          </cell>
+          <cell r="G36" t="str">
+            <v xml:space="preserve"> Reisa Džemaludina Čauševića 1, 71000 Sarajevo     </v>
+          </cell>
+          <cell r="H36" t="str">
+            <v>https://mo.ks.gov.ba/kontakti</v>
+          </cell>
+          <cell r="I36">
+            <v>38733562128</v>
+          </cell>
+          <cell r="J36" t="str">
+            <v xml:space="preserve">mo@mo.ks.gov.ba </v>
+          </cell>
+          <cell r="K36" t="str">
+            <v>Zakon o osnovnom odgoju i obrazovanju (Službene novine Kantona Sarajevo, 23/2017, 33/2017, 30/2019, 34/2020, 33/2021)
+Pravilnik o inkluzivnom obrazovanju (Službene novine Kantona Sarajevo, 32/19)</v>
+          </cell>
+          <cell r="L36" t="str">
+            <v>Nije definisan; Nema upute kako "započeti" proces za roditelja/dijete. Definirano je da ustanova/centar treba da se obrati ministarstvu za dodatnu podršku, ministarstvo rješava zahtjeve (prema obrascu) za 15 dana.</v>
+          </cell>
+          <cell r="M36" t="str">
+            <v>Nije definisano</v>
+          </cell>
+          <cell r="N36" t="str">
+            <v>N/a</v>
+          </cell>
+          <cell r="P36" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>Usluge centara za prevenciju</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v>Logopedi, defektolozi</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob</v>
+          </cell>
+          <cell r="E37" t="str">
+            <v>Zdravstvena zaštita</v>
+          </cell>
+          <cell r="K37" t="str">
+            <v>Zakon o osnovama socijalne zaštite, zaštite civilnih žrtava rata i zaštite porodice s djecom, Član 88: Zaštita porodice sa djecom ima za cilj:
+da se osiguraju svoj djeci približno jednaki uvjeti za zdrav i pravilan tjelesni, intelektualni i emocionalni razvoj u porodici,
+pomoć u ostvarivanju njene reproduktivne uloge, njezi, podizanju, odgoju i zaštiti djece i poboljšanju kvaliteta života porodice,
+razvijanje humanih odnosa u skladu sa načelima građanskog morala i solidarnosti.
+Djetetu bez oba ili jednog roditelja, porodici koja ima dijete ometeno u fizičkom ili psihičkom razvoju i porodici u kojoj su oba ili jedan roditelj invalidi, osiguravaju se povoljniji uvjeti u sticanju i ostvarivanju prava i veći iznosi materijalnih i drugih davanja utvrđenih ovim zakonom i propisom kantona.</v>
+          </cell>
+          <cell r="P37" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Jednokratna novčana pomoć za invalidna lica</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v>Općina Ilidža: Općinski načelnik dodjeljuje jednokratnu novčanu pomoć osobama sa invaliditetom sa posebnim potrebama koje su u socijalnoj potrebi.</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="E38" t="str">
+            <v>Socijalna zaštita za PwD</v>
+          </cell>
+          <cell r="F38" t="str">
+            <v>Općina Ilidža</v>
+          </cell>
+          <cell r="G38" t="str">
+            <v>Butmirska cesta 12, prvi sprat</v>
+          </cell>
+          <cell r="H38" t="str">
+            <v>https://www.opcinailidza.ba/services/sluzba-za-socijalna-pitanja-zdravstvo-izbjeglice-i-raseljena-lica</v>
+          </cell>
+          <cell r="I38">
+            <v>387733637384</v>
+          </cell>
+          <cell r="J38" t="str">
+            <v>sejda.topalovic@opcinailidza.ba</v>
+          </cell>
+          <cell r="K38" t="str">
+            <v>Pomoć se dodjeljuje kontinuirano posljednjih 10 godina</v>
+          </cell>
+          <cell r="L38" t="str">
+            <v>Dodjela se vrši na osnovu evidencija Službe, a upis u evidenciju  može se izvršti i na način da se dostavi  dokumentacija Službi za socijalna pitanja, zdravstvo, izbjeglice i raseljena lica Općine Ilidža na adresi Butmirska cesta 12, -prvi sprat</v>
+          </cell>
+          <cell r="M38" t="str">
+            <v>CIPS-ova prijava mjesta boravka
+Rješenje koje je doneseno u skladu Pravilnikom o utvrđivanju preostale sposobnosti i razvrstavanju djece i omladine ometene u psiho-fizičkom razvoju ("Službene novine Kantona Sarajevo" br. 26/08 i 5/12), odnsono medicinskom dokumentacijom za djecu oboljelu od od karcinoma, šećerne bolesti, leukemije, TBC i celijakije</v>
+          </cell>
+          <cell r="N38" t="str">
+            <v>ZAHTJEV ZA PRIZNAVANJE PRAVA NA JEDNOKRATNU NOVČANU POMOĆ I SUFINANSIRANJE MEDICINSKI POTPOMOGNUTE OPLODNJE.pdf (opcinailidza.ba)</v>
+          </cell>
+          <cell r="P38" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Jednokratna novčana pomoć za stanovnike starije od 80 godina</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>Jednokratna novčana pomoć koja se godišnje dodjeljuje svim stanovnicima opštine starijim od 80 godina. Iznos zavisi od raspoloživosti sredstava u budžetu.</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>Treća životna dob</v>
+          </cell>
+          <cell r="E39" t="str">
+            <v>Elderly</v>
+          </cell>
+          <cell r="F39" t="str">
+            <v>Općina Ilidža</v>
+          </cell>
+          <cell r="G39" t="str">
+            <v>Butmirska cesta 12, prvi sprat</v>
+          </cell>
+          <cell r="I39">
+            <v>387733637384</v>
+          </cell>
+          <cell r="J39" t="str">
+            <v>sejda.topalovic@opcinailidza.ba</v>
+          </cell>
+          <cell r="K39" t="str">
+            <v>Raspodjela na osnovu evidencije mjesnih zajednica</v>
+          </cell>
+          <cell r="L39" t="str">
+            <v>N/a</v>
+          </cell>
+          <cell r="M39" t="str">
+            <v>N/a</v>
+          </cell>
+          <cell r="N39" t="str">
+            <v>N/a</v>
+          </cell>
+          <cell r="P39" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>Jednokratna novčana pomoć za teško bolesne osobe i umjetnu oplodnju</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>Novčana pomoć za teško oboljela lica sa područja općine Ilidža kojima je potrebno plaćanje troškova liječenja u zemlji i/ili inostranstvu.</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="E40" t="str">
+            <v>Zdravstvena zaštita</v>
+          </cell>
+          <cell r="F40" t="str">
+            <v>Općina Ilidža</v>
+          </cell>
+          <cell r="G40" t="str">
+            <v>Butmirska cesta 12, prvi sprat</v>
+          </cell>
+          <cell r="H40" t="str">
+            <v>ZAHTJEV ZA PRIZNAVANJE PRAVA NA JEDNOKRATNU NOVČANU POMOĆ I SUFINANSIRANJE MEDICINSKI POTPOMOGNUTE OPLODNJE.pdf (opcinailidza.ba)</v>
+          </cell>
+          <cell r="I40">
+            <v>387733637384</v>
+          </cell>
+          <cell r="J40" t="str">
+            <v>sejda.topalovic@opcinailidza.ba</v>
+          </cell>
+          <cell r="K40" t="str">
+            <v>Za rješavanje zahtjeva nadležna je Komisija koju čine ljekari različitih specijalnosti</v>
+          </cell>
+          <cell r="L40" t="str">
+            <v>ZAHTJEV ZA PRIZNAVANJE PRAVA NA JEDNOKRATNU NOVČANU POMOĆ I SUFINANSIRANJE MEDICINSKI POTPOMOGNUTE OPLODNJE.pdf (opcinailidza.ba)</v>
+          </cell>
+          <cell r="M40" t="str">
+            <v>ZAHTJEV ZA PRIZNAVANJE PRAVA NA JEDNOKRATNU NOVČANU POMOĆ I SUFINANSIRANJE MEDICINSKI POTPOMOGNUTE OPLODNJE.pdf (opcinailidza.ba)</v>
+          </cell>
+          <cell r="N40" t="str">
+            <v>ZAHTJEV ZA PRIZNAVANJE PRAVA NA JEDNOKRATNU NOVČANU POMOĆ I SUFINANSIRANJE MEDICINSKI POTPOMOGNUTE OPLODNJE.pdf (opcinailidza.ba)</v>
+          </cell>
+          <cell r="P40" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>Oslobađanje od plaćanja RTV takse za osobe koje su izgubile sluh i vid</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>Od obaveze plaćanja RTV takse oslobađaju se vlasnici prijemnika koji su trajno izgubili vid ili sluh i žive sami u domaćinstvu ili sa starateljem.</v>
+          </cell>
+          <cell r="F41" t="str">
+            <v>Radio–televizija Bosne i Hercegovine</v>
+          </cell>
+          <cell r="G41" t="str">
+            <v>Bulevar Meše Selimovića 12</v>
+          </cell>
+          <cell r="L41" t="str">
+            <v>Zahtjev za ostvarenje prava podnosi se Radio–televiziji Bosne i Hercegovine u Sarajevu.</v>
+          </cell>
+          <cell r="M41" t="str">
+            <v>Zahtjev
+Kopija lične karte
+Kućna lista
+Dokument o starateljstvu koji izdaje centar za socijalni rad u mjestu prebivališta
+Kopiju lične karte;
+Kućnu listu;
+Dokument o starateljstvu (ako ga imate) koji izdaje centar za socijalni rad u mjestu prebivališta</v>
+          </cell>
+          <cell r="P41" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>Oslobađanje plaćanja  uvoznih dadžbina, carine i PDV-a prilikom uvoza automobila</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>Osobe s invaliditetom i poteškoćama u razvoju mogu biti oslobođene plaćanja uvoznih dadžbina, odnosno carine i PDV-a, ako planiraju kupiti i uvesti automobil koji će im poslužiti kao ortopedsko ili drugo pomagalo.
+Pravo na oslobađanje odnosi se na period od pet godina, što znači nakon uvoza vozila na ovaj način, u narednih pet godina ne mogu na isti način uvesti vozilo. Tek nakon isteka perioda od pet godina mogu ponovo na povlasticu uvesti vozilo. Isto tako, vozilo ne smiju prodati u trajanju od tri godine od dana uvoza, jer ako to urade moraju platiti sve uvozne dažbine.
+Invalidna osoba može uvesti putnički automobil do vrijednosti od 30.000 KM ako nije posebno prilagođen za upravljanje invalidnih osoba ili bez ograničenja vrijednosti ako se uvozi putnički automobil posebno prilagođen za prijevoz invalidnih osoba.</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="E42" t="str">
+            <v>Prevoz</v>
+          </cell>
+          <cell r="F42" t="str">
+            <v>MUP Kantona Sarajevo</v>
+          </cell>
+          <cell r="L42" t="str">
+            <v>Zahtjev za oslobadjanje od plaćanja carine podnosi se nadležnoj carinskoj upravi</v>
+          </cell>
+          <cell r="M42" t="str">
+            <v>- nalaz ocjena ili mišljenje o stepenu oštećenja ekstremiteta bitnog za upravljanje vozilom izdatog od strane organa entiteta, BiH i Brčko distrikta BiH,
+- dvije fotografije dimenzija 30 s 35 mm,
+- lična karta na uvid i
+- fotokopija potvrde o vlasništvu nad motornim vozilom.</v>
+          </cell>
+          <cell r="P42" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>Osnovna dijagnostika</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>Osobe s invaliditetom imaju pravo na besplatnu osnovnu dijagnostiku na KCUS-u i Domovizma zdravlja KS.</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="E43" t="str">
+            <v>Zdravstvena zaštita</v>
+          </cell>
+          <cell r="F43" t="str">
+            <v>Klinički centar Univerziteta u Sarajevu i Domovi zdravlja Kantona Sarajevo</v>
+          </cell>
+          <cell r="P43" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44" t="str">
+            <v xml:space="preserve">Osnovni paket fiksne telefonije - socijalni </v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>Pravo na Socijalni paket ostvaruju: porodice palog borca, ratni vojni invalidi sa 100% invalidnosti, slijepa lica i kategorije, lica oboljela od distrofije i srodnih bolesti, paraplegičari, oboljeli od dječje ili cerebralne paralize i multiple skleroze i korisnici stalne novčane pomoći, u smislu zakona o osnovama socijalne zaštite, zaštite civilnih žrtava rata i zaštite porodica sa djecom i odgovarajućih kantonalnih pozitivnih propisa u FBiH, kojima se uređuje ova oblast.</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="F44" t="str">
+            <v>BH Telecom</v>
+          </cell>
+          <cell r="G44" t="str">
+            <v>Zmaja od Bosne 88</v>
+          </cell>
+          <cell r="H44" t="str">
+            <v>https://mojwebshop.bhtelecom.ba/INTERSHOP/web/BOS/BHTelecomWebShop-BHTelecom-Site/bs_BA/-/BAM/ViewProduct-Start?SKU=100003</v>
+          </cell>
+          <cell r="I44">
+            <v>38733653093</v>
+          </cell>
+          <cell r="P44" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45" t="str">
+            <v>Porez na dohodak, umanjenje poreza na zaposlene osobe sa invaliditetom</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v xml:space="preserve">Zaposlene osobe s invaliditetom imaju pravo na osnovni lični odbitak i umanjenje porezne osnovice po osnovu izdražavanja članova uže porodice i /ili po osnovu eventualne invalidnosti tih članova ili samog poreznog obveznika.
+Rezidentni porezni obveznici mogu odbiti i lični odbitak: 0,3 osnovnog ličnog odbitka iz stava (1) člana 24 za utvrđenu vlastitu invalidnost, kao i za utvrđenu invalidnost svakog člana uže porodice koje porezni obveznik izdržava. </v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="E45" t="str">
+            <v>Poreske olakšice</v>
+          </cell>
+          <cell r="F45" t="str">
+            <v>Poreska uprava Općine</v>
+          </cell>
+          <cell r="K45" t="str">
+            <v>Zakn o porezu na dohodak FBiH</v>
+          </cell>
+          <cell r="M45" t="str">
+            <v>Kopija lične karte
+Vjenčani list;
+Rodni list;
+Dokaz o visini prihoda izdržavanog lica;
+Uvjerenje o zajedničkom domaćinstvu;
+Rješenje nadležnog organa sa utvrđenim tjelesnim oštećenjem i stepena invaliditeta</v>
+          </cell>
+          <cell r="P45" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46" t="str">
+            <v xml:space="preserve">Posebna ishrana </v>
+          </cell>
+          <cell r="D46" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob; Radni vijek; Treća životna dob</v>
+          </cell>
+          <cell r="F46" t="str">
+            <v>Zavod zdravstvenog osiguranja KS</v>
+          </cell>
+          <cell r="P46" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47" t="str">
+            <v>Povlastice u željezničkom saobraćaju</v>
+          </cell>
+          <cell r="K47" t="str">
+            <v>http://www.sluzbenilist.ba/page/akt/lbKAkKGaEwg=</v>
+          </cell>
+          <cell r="P47" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48" t="str">
+            <v>Pravo na druge primjerene oblike pomoći djeci u predškolskim ustanovama, redovnim osnovnim i srednjim školama i ustanovama osnovnoškolskog i srednjoškolskog odgoja obrazovanja i rehabilitacije za učenike sa teškoćama (ustanove): 
+a.	Program edukacijsko rehabilitacijskih tretmana
+b.	Program produženog stručnog postupka
+c.	Rehabilitacijski programi</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>Program edukacijsko-rehabilitacijskih tretmana sastoji se od posebnih defektoloških/edukacijsko-rehabilitacijskih sadržaja koji se različitim postupcima provode u svrhu uspješnijeg usvajanja nastavnih sadržaja kao i za pospješivanje boljeg fukncioniranja.</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v>Školska dob</v>
+          </cell>
+          <cell r="L48" t="str">
+            <v>Nije definisan; Nema upute kako "započeti" proces za roditelja/dijete. Definirano je da ustanova/centar treba da se obrati ministarstvu za dodatnu podršku, ministarstvo rješava zahtjeve (prema obrascu) za 15 dana.</v>
+          </cell>
+          <cell r="P48" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49" t="str">
+            <v>Pravo na individualni prilagođeni program (IPP) – IPP1 IPP2 IPP3</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v xml:space="preserve">IPP je dokument koji se odnosi na sadržajno i metodičko prilagođavanje u radu s djecom. Uključuje prilagođavanje sadržaja djetetovim mogućnostima. Prilagođenim programom, specifičnim za svakog učenika (prilagođavanje, prvenstevno sposobnostima, mogućnostima i potrebama) utvrđuje se oblik i nivo podrške u oblasti akademskih i vanakademskih znanja i vještina, vrijeme i trajanje podrške, kao i kriteriji, sredstva i metode vrednovanja uspješnosti u učenju i socijalnim i drugim područjima funkcioniranja djeteta. Izrađuje se u situaciji kada je stepen teškoće takav da dijete ne može isti savladati čak ni programom koji traži minimalne programske zahtjeve. </v>
+          </cell>
+          <cell r="D49" t="str">
+            <v>Školska dob</v>
+          </cell>
+          <cell r="E49" t="str">
+            <v>Obrazovanje</v>
+          </cell>
+          <cell r="F49" t="str">
+            <v>Ministarstvo odgoja i obrazovanja</v>
+          </cell>
+          <cell r="G49" t="str">
+            <v xml:space="preserve">Reisa Džemaludina Čauševića 1, 71000 Sarajevo     </v>
+          </cell>
+          <cell r="H49" t="str">
+            <v>https://mo.ks.gov.ba/kontakti</v>
+          </cell>
+          <cell r="I49">
+            <v>38733562128</v>
+          </cell>
+          <cell r="J49" t="str">
+            <v xml:space="preserve">mo@mo.ks.gov.ba </v>
+          </cell>
+          <cell r="K49" t="str">
+            <v>Zakon o osnovnom odgoju i obrazovanju (Službene novine Kantona Sarajevo, 23/2017, 33/2017, 30/2019, 34/2020, 33/2021)
+Pravilnik o inkluzivnom obrazovanju (Službene novine Kantona Sarajevo, 32/19)</v>
+          </cell>
+          <cell r="L49" t="str">
+            <v>Nije definisan; Nema upute kako "započeti" proces za roditelja/dijete. Definirano je da ustanova/centar treba da se obrati ministarstvu za dodatnu podršku, ministarstvo rješava zahtjeve (prema obrascu) za 15 dana.</v>
+          </cell>
+          <cell r="M49" t="str">
+            <v>Nije definisano</v>
+          </cell>
+          <cell r="N49" t="str">
+            <v>N/a</v>
+          </cell>
+          <cell r="P49" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50" t="str">
+            <v>Pravo na pelene</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v>Novorođenče</v>
+          </cell>
+          <cell r="F50" t="str">
+            <v>Zavod zdravstvenog osiguranja KS</v>
+          </cell>
+          <cell r="P50" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51" t="str">
+            <v>Pružanje oralno-hirurških i stomatoloških usluga za djecu sa poteškoćama u razvoju</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v>Na Stomatološkom fakultetu u Sarajevu djeci s poteškoćama u razvoju pružaju se besplatne oralnohirurške i stomatološke usluge, ako je potrebno i pod općom anestezijom. .</v>
+          </cell>
+          <cell r="D51" t="str">
+            <v>Predškolska dob; Školska dob</v>
+          </cell>
+          <cell r="E51" t="str">
+            <v>Zdravstvena zaštita</v>
+          </cell>
+          <cell r="F51" t="str">
+            <v>Stomatološki fakultet u Sarajevu</v>
+          </cell>
+          <cell r="G51" t="str">
+            <v>Bolnička 4, Sarajevo</v>
+          </cell>
+          <cell r="H51" t="str">
+            <v>https://sf.unsa.ba/pruzanje-oralno-hirurskih-i-stomatoloskih-usluga-za-djecu-sa-poteskocama-u-razvoju/</v>
+          </cell>
+          <cell r="I51">
+            <v>38733214249</v>
+          </cell>
+          <cell r="M51" t="str">
+            <v>https://sf.unsa.ba/pruzanje-oralno-hirurskih-i-stomatoloskih-usluga-za-djecu-sa-poteskocama-u-razvoju/</v>
+          </cell>
+          <cell r="N51" t="str">
+            <v>https://sf.unsa.ba/pruzanje-oralno-hirurskih-i-stomatoloskih-usluga-za-djecu-sa-poteskocama-u-razvoju/</v>
+          </cell>
+          <cell r="P51" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52" t="str">
+            <v>Subvencija  za djecu istih roditelja - oslobađanje plaćanja vrtića za braću i sestre djeteta sa poteškoćama u razvoju</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v>Djeca koja su braća/sestre djeteta sa poteškoćama u razvoju imaju pravo na subvenciju troškova vrtića.</v>
+          </cell>
+          <cell r="D52" t="str">
+            <v>Predškolska dob;</v>
+          </cell>
+          <cell r="E52" t="str">
+            <v>Obrazovanje</v>
+          </cell>
+          <cell r="F52" t="str">
+            <v>Općinski nivo</v>
+          </cell>
+          <cell r="P52" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53" t="str">
+            <v>Ugradnja inzulinske pumpice</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v xml:space="preserve">Osigurana lica - djeca do 18 godina, inzuloovisnici, na prijedlog tima za inzulinske pumpe pedijatrijske klinike, a uz odobrenje komisije Zavoda, mogu ostvariti pravo na inzulinsku pumpu. Uz inzulinsku pumpu obezbješuje se potrošni materijal: </v>
+          </cell>
+          <cell r="D53" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob</v>
+          </cell>
+          <cell r="E53" t="str">
+            <v>Zdravstvena zaštita</v>
+          </cell>
+          <cell r="F53" t="str">
+            <v>Zavod zdravstvenog osiguranja KS</v>
+          </cell>
+          <cell r="K53" t="str">
+            <v>Uredba o obimu, uvjetima i načiu ostvarivanja prava osiguranih lica na korištenje ortopedskih i drugih pomagala, endoproteza, stomatološko protetske pomoći i stomatološko - protetskih nadomjestaka
+https://www.kzzosa.ba/wp-content/uploads/2023/08/Odluka_o_visini_ucesca_ZZO_KS_u_cijeni_medicinskih_sredstava-1.pdf</v>
+          </cell>
+          <cell r="P53" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54" t="str">
+            <v>Uvećani dječiji doplatak</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v>Ako je neki član porodice lice sa invaliditetom, djeca imaju pravo na uvećani dječiji dodatak. Zakonom nije predviđen imovinski cenzus. 
+Obratiti se nadležnoj službi u općini stanovanja, popuniti zahtjev i priložiti tražene dokumente.</v>
+          </cell>
+          <cell r="D54" t="str">
+            <v>Novorođenče; Predškolska dob; Školska dob</v>
+          </cell>
+          <cell r="E54" t="str">
+            <v>Socijalna zaštita</v>
+          </cell>
+          <cell r="F54" t="str">
+            <v>Općine</v>
+          </cell>
+          <cell r="P54" t="str">
+            <v>Prava, nasumični postupci</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="18">
+        <row r="1">
+          <cell r="E1" t="str">
+            <v>Novorođenče</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="E2" t="str">
+            <v>Ambulanta "Sve na jednom mjestu" za djecu i osobe s poteškoćama u razvoju</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="E3" t="str">
+            <v>Dodatak za njegu i pomoć od strane drugog lica, Civilne žrtve rata</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4" t="str">
+            <v>Jednokratna novčana pomoć licima i domaćinstvima sa područja općine Novo Sarajevo</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5" t="str">
+            <v>Jednokratna novčana pomoć za invalidna lica</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="E6" t="str">
+            <v>Jednokratna novčana pomoć za teško bolesne osobe i umjetnu oplodnju</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7" t="str">
+            <v>Kupovina lijekova po posebnim protokolima</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>Medicinska rehabilitacija/banjsko liječenje kao produženo bolničko liječenje</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9" t="str">
+            <v>Medicinska sredstva - ortopedska pomagala</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10" t="str">
+            <v>Ocjenjivanje sposobnosti, razvrstavanje djece i omladine ometene u psiho-fizičkom razvoju</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11" t="str">
+            <v>Osnovna dijagnostika</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="E12" t="str">
+            <v xml:space="preserve">Osnovni paket fiksne telefonije - socijalni </v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13" t="str">
+            <v>Porez na dohodak, umanjenje poreza na zaposlene osobe sa invaliditetom</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="E14" t="str">
+            <v xml:space="preserve">Posebna ishrana </v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="E15" t="str">
+            <v>Pravo na kućnu njegu</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="E16" t="str">
+            <v>Pravo na ličnu invalidninu, dodatak za njegu i pomoć drugog lica i ortopedski dodatak</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="E17" t="str">
+            <v>Pravo na pelene</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="E18" t="str">
+            <v>Pravo na penziju</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="E19" t="str">
+            <v>Pravo na stalnu novčanu pomoć</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="E20" t="str">
+            <v>Pravo na zdravstvenu zaštitu</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="E21" t="str">
+            <v>Pravo roditelja njegovatelja na osiguranje</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="E22" t="str">
+            <v>Pravo roditelja njegovatelja na pokrivanje troškova sahrane/dženaze</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="E23" t="str">
+            <v>Prednost u primanju usluga u zdravstvenom i drugim institucijama</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="E24" t="str">
+            <v>Priznavanje statusa roditelja njegovatelja</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="E25" t="str">
+            <v>Refundacija troškova lijekova i liječenja</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="E26" t="str">
+            <v>Smještaj u hospis</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="E27" t="str">
+            <v>Smještaj u ustanovu, njega, rehabilitacija i socijalna zaštita – Dom za djecu bez roditeljskog staranja</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="E28" t="str">
+            <v>Ugradnja inzulinske pumpice</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="E29" t="str">
+            <v>Usluge centara za prevenciju</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="E30" t="str">
+            <v>Uvećani dječiji doplatak</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Amra Kapo" id="{FE1FD6E1-A811-4748-8FA2-0CB75D7C2C7E}" userId="55206a9b6e884185" providerId="Windows Live"/>
@@ -10818,70 +11964,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F8E5540E-A15D-4EBA-B54B-F2677BCFD519}" name="Table6" displayName="Table6" ref="A1:F11" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
-  <autoFilter ref="A1:F11" xr:uid="{F8E5540E-A15D-4EBA-B54B-F2677BCFD519}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3CD3A6FA-48B3-4742-8A53-DD72379ADF8D}" name="Naziv " dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{822BDE87-6F30-4A0E-A5E2-A9CA37AF424B}" name="Opis" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{58D77055-6C4D-4085-8930-2E537F7B48A2}" name="Životna dob" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{63ED1170-2807-4400-9BED-30ED8580EBF4}" name="Pravni osnov" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{EDBC30B4-6F48-4A07-8E16-A1D618F93B57}" name="Pojašnjenje (Član)" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{97503B81-1CB4-45AC-A9F3-58BBE73723CB}" name="Web stranica" dataDxfId="46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F8E5540E-A15D-4EBA-B54B-F2677BCFD519}" name="Table6" displayName="Table6" ref="A1:H10" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+  <autoFilter ref="A1:H10" xr:uid="{F8E5540E-A15D-4EBA-B54B-F2677BCFD519}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3CD3A6FA-48B3-4742-8A53-DD72379ADF8D}" name="Naziv " dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{822BDE87-6F30-4A0E-A5E2-A9CA37AF424B}" name="Opis" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{58D77055-6C4D-4085-8930-2E537F7B48A2}" name="Životna dob" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{63ED1170-2807-4400-9BED-30ED8580EBF4}" name="Pravni osnov" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{EDBC30B4-6F48-4A07-8E16-A1D618F93B57}" name="Pojašnjenje (Član)" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{97503B81-1CB4-45AC-A9F3-58BBE73723CB}" name="Web stranica" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{646B6EF2-2411-4AC8-BDB0-4AF11327443D}" name="Lat" dataDxfId="6">
+      <calculatedColumnFormula>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{625BAEF3-1CEB-40FC-B187-7825789CE907}" name="Lon" dataDxfId="5">
+      <calculatedColumnFormula>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC01B4FA-5515-495E-8493-A665299851AA}" name="Table2" displayName="Table2" ref="A1:Q31" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="A1:Q31" xr:uid="{DC01B4FA-5515-495E-8493-A665299851AA}"/>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{1F9E85E2-0B42-4580-82E0-6EEF465356B7}" name="#" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{4219DB81-11D2-48FE-B7E2-5608FFF50B55}" name="Naziv " dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{694A58F1-2A0C-4062-B856-7D3DE3AB2B87}" name="Opis" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{E6B32774-7F5A-4404-BA91-DAEFC1C6DC74}" name="Životna dob" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{F53571F7-E67A-4D75-B971-A9E579E334CE}" name="Godine" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{C56B24ED-F555-4C1E-8F1F-95E0A9F19EBD}" name="Tip usluge/prava/benefita" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{E061CC34-19FF-417C-8134-E10A7AFAB410}" name="Institucija" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{772F549A-88E3-465F-A720-D9DB53E72F53}" name="Adresa" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{4CEF74C2-07E0-4B89-85D3-C9E9B9A1743A}" name="Web stranica" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{DF65403C-1AF1-4456-B8F7-E59BD4641A90}" name="Telefon" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{691CF05D-6BDD-4AAD-97E1-9C52B75F2E41}" name="Email" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{AE92B2E5-DC89-43B9-A62F-8B64611EDD93}" name="Pravni osnov" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{6CEED575-5B30-4A77-AB59-1EC60905A98A}" name="Proces aplikacije" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{FFE031DC-1278-4B8E-AE6A-C8D486B3F7DB}" name="Lista neophodnih dokumenata" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{A3CB64C4-787A-4D5D-A31E-037D47BCA561}" name="Link za informacije o prijavi" dataDxfId="26"/>
-    <tableColumn id="16" xr3:uid="{2A4E65B2-B182-44CE-8C1E-844CC2177CFC}" name="Vremenski okvir" dataDxfId="25"/>
-    <tableColumn id="17" xr3:uid="{D7268B50-AA0A-4678-B0CA-B96626BF4CE7}" name="Dodatne napomene" dataDxfId="24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC01B4FA-5515-495E-8493-A665299851AA}" name="Table2" displayName="Table2" ref="A1:S31" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="A1:S31" xr:uid="{DC01B4FA-5515-495E-8493-A665299851AA}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{1F9E85E2-0B42-4580-82E0-6EEF465356B7}" name="#" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{4219DB81-11D2-48FE-B7E2-5608FFF50B55}" name="Naziv " dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{694A58F1-2A0C-4062-B856-7D3DE3AB2B87}" name="Opis" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{E6B32774-7F5A-4404-BA91-DAEFC1C6DC74}" name="Životna dob" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{F53571F7-E67A-4D75-B971-A9E579E334CE}" name="Godine" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{C56B24ED-F555-4C1E-8F1F-95E0A9F19EBD}" name="Tip usluge/prava/benefita" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{E061CC34-19FF-417C-8134-E10A7AFAB410}" name="Institucija" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{772F549A-88E3-465F-A720-D9DB53E72F53}" name="Adresa" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{4CEF74C2-07E0-4B89-85D3-C9E9B9A1743A}" name="Web stranica" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{DF65403C-1AF1-4456-B8F7-E59BD4641A90}" name="Telefon" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{691CF05D-6BDD-4AAD-97E1-9C52B75F2E41}" name="Email" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{AE92B2E5-DC89-43B9-A62F-8B64611EDD93}" name="Pravni osnov" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{6CEED575-5B30-4A77-AB59-1EC60905A98A}" name="Proces aplikacije" dataDxfId="32"/>
+    <tableColumn id="14" xr3:uid="{FFE031DC-1278-4B8E-AE6A-C8D486B3F7DB}" name="Lista neophodnih dokumenata" dataDxfId="31"/>
+    <tableColumn id="15" xr3:uid="{A3CB64C4-787A-4D5D-A31E-037D47BCA561}" name="Link za informacije o prijavi" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{2A4E65B2-B182-44CE-8C1E-844CC2177CFC}" name="Vremenski okvir" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{D7268B50-AA0A-4678-B0CA-B96626BF4CE7}" name="Dodatne napomene" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{D7CC9E88-F8AA-4482-A4F3-AFF654B37299}" name="Lat" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{E212D38E-3C14-4451-9823-9825AA7C6B45}" name="Lon" dataDxfId="7">
+      <calculatedColumnFormula>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5FC73C86-88F7-4509-A95A-5168F4D44A8C}" name="Table5" displayName="Table5" ref="A1:N18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5FC73C86-88F7-4509-A95A-5168F4D44A8C}" name="Table5" displayName="Table5" ref="A1:N18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{93C9BA4B-E353-4D19-A8B1-FD649D881751}" name="Naziv " dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{37CD3CA4-A5B4-48AA-8EAB-A634118E07F6}" name="Opis" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{166DA75C-3FDE-4343-A1C5-D2960F08F3B9}" name="Tip usluge/prava/benefita" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{7400F049-A05D-4A4E-99A4-43B56FBA226C}" name="Životna dob" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{762D7820-5F72-4954-AFF5-8563D1F25EDF}" name="Korisnici" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{037E89ED-4586-4EB8-8009-1DC090C06F9E}" name="Ministartvo/Organizacija" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{2DE3B312-9D8F-4CF9-8624-2A6E25D376D2}" name="Adresa" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{F2FDB37F-57A2-4F5E-8AE1-29D816260855}" name="Web stranica" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{9507BFE2-DD4B-41AE-A7ED-EE3EA04689F9}" name="Telefon" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{422D2703-FD84-4A66-A590-54DC013958FF}" name="Email" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{7DAAC0A0-5795-416B-8172-BF7FB16CF71C}" name="Pravni okvir" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{3FECE412-1757-4D30-BE43-D03589D55C54}" name="Proces aplikacije" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{9CCCC0FB-8F10-4A5D-BA9F-34BEB2AACEA9}" name="Lista neophodnih dokumenata" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{897F94AA-266F-4177-BC01-F1BA673F652B}" name="Link za informacije o prijavi" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{93C9BA4B-E353-4D19-A8B1-FD649D881751}" name="Naziv " dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{37CD3CA4-A5B4-48AA-8EAB-A634118E07F6}" name="Opis" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{166DA75C-3FDE-4343-A1C5-D2960F08F3B9}" name="Tip usluge/prava/benefita" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{7400F049-A05D-4A4E-99A4-43B56FBA226C}" name="Životna dob" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{762D7820-5F72-4954-AFF5-8563D1F25EDF}" name="Korisnici" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{037E89ED-4586-4EB8-8009-1DC090C06F9E}" name="Ministartvo/Organizacija" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{2DE3B312-9D8F-4CF9-8624-2A6E25D376D2}" name="Adresa" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{F2FDB37F-57A2-4F5E-8AE1-29D816260855}" name="Web stranica" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{9507BFE2-DD4B-41AE-A7ED-EE3EA04689F9}" name="Telefon" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{422D2703-FD84-4A66-A590-54DC013958FF}" name="Email" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{7DAAC0A0-5795-416B-8172-BF7FB16CF71C}" name="Pravni okvir" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{3FECE412-1757-4D30-BE43-D03589D55C54}" name="Proces aplikacije" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{9CCCC0FB-8F10-4A5D-BA9F-34BEB2AACEA9}" name="Lista neophodnih dokumenata" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{897F94AA-266F-4177-BC01-F1BA673F652B}" name="Link za informacije o prijavi" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E703D76D-D302-4320-BEB5-A55625437D7F}" name="Zivotnadob" displayName="Zivotnadob" ref="D1:D5" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E703D76D-D302-4320-BEB5-A55625437D7F}" name="Zivotnadob" displayName="Zivotnadob" ref="D1:D5" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="D1:D5" xr:uid="{E703D76D-D302-4320-BEB5-A55625437D7F}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{5BD196D3-17BC-4525-A2D1-C125915FE5E4}" name="Životna dob"/>
@@ -11459,7 +12617,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="str" cm="1">
-        <f t="array" ref="C1">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$98,ISNUMBER(SEARCH("Novorođenče",'Neinstitucionalizirana prava'!$C$2:$C$98)), "0")</f>
+        <f t="array" ref="C1">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$97,ISNUMBER(SEARCH("Novorođenče",'Neinstitucionalizirana prava'!$C$2:$C$97)), "0")</f>
         <v>0</v>
       </c>
       <c r="D1" t="str" cm="1">
@@ -11471,7 +12629,7 @@
         <v>Ambulanta "Sve na jednom mjestu" za djecu i osobe s poteškoćama u razvoju</v>
       </c>
       <c r="F1" t="str" cm="1">
-        <f t="array" ref="F1:F3">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$98,ISNUMBER(SEARCH("Predškolska dob",'Neinstitucionalizirana prava'!$C$2:$C$98)),"0")</f>
+        <f t="array" ref="F1:F3">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$97,ISNUMBER(SEARCH("Predškolska dob",'Neinstitucionalizirana prava'!$C$2:$C$97)),"0")</f>
         <v>Pravo na penziju korsnika ili roditelja/staratelja</v>
       </c>
       <c r="G1" s="13" t="str" cm="1">
@@ -11483,7 +12641,7 @@
         <v>Ambulanta "Sve na jednom mjestu" za djecu i osobe s poteškoćama u razvoju</v>
       </c>
       <c r="I1" s="13" t="str" cm="1">
-        <f t="array" ref="I1:I6">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$98,ISNUMBER(SEARCH("Školska dob",'Neinstitucionalizirana prava'!$C$2:$C$98)),"0")</f>
+        <f t="array" ref="I1:I6">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$97,ISNUMBER(SEARCH("Školska dob",'Neinstitucionalizirana prava'!$C$2:$C$97)),"0")</f>
         <v>Pravo na dnevni boravak u posebnim ustanovama ili smještaj u domovima tokom obrazovanja. Potpuno pokriće troškova dnevnog boravka od strane Centra</v>
       </c>
       <c r="J1" t="str" cm="1">
@@ -11495,7 +12653,7 @@
         <v>Ambulanta "Sve na jednom mjestu" za djecu i osobe s poteškoćama u razvoju</v>
       </c>
       <c r="L1" t="str" cm="1">
-        <f t="array" ref="L1:L6">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$98,ISNUMBER(SEARCH("Radni vijek",'Neinstitucionalizirana prava'!$C$2:$C$98)),"0")</f>
+        <f t="array" ref="L1:L6">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$97,ISNUMBER(SEARCH("Radni vijek",'Neinstitucionalizirana prava'!$C$2:$C$97)),"0")</f>
         <v>Pravo na kućnu njegu</v>
       </c>
       <c r="M1" s="13" t="str" cm="1">
@@ -11507,7 +12665,7 @@
         <v>Ambulanta "Sve na jednom mjestu" za djecu i osobe s poteškoćama u razvoju</v>
       </c>
       <c r="O1" s="13" t="str" cm="1">
-        <f t="array" ref="O1">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$98,ISNUMBER(SEARCH("Treća životna dob",'Neinstitucionalizirana prava'!$C$2:$C$98)),"0")</f>
+        <f t="array" ref="O1">_xlfn._xlws.FILTER('Neinstitucionalizirana prava'!$A$2:$A$97,ISNUMBER(SEARCH("Treća životna dob",'Neinstitucionalizirana prava'!$C$2:$C$97)),"0")</f>
         <v>Pravo na kućnu njegu</v>
       </c>
     </row>
@@ -12011,6 +13169,151 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6717636-9D63-4CEF-B4BB-541077ED8170}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="B2:H17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" style="10"/>
+    <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="76" style="15" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="77.5546875" style="125" customWidth="1"/>
+    <col min="6" max="8" width="14.88671875" style="125" customWidth="1"/>
+    <col min="9" max="16384" width="8.5546875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="14.4">
+      <c r="B2"/>
+    </row>
+    <row r="3" spans="2:8" ht="14.4">
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="2:8" ht="14.4">
+      <c r="B4"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.4" thickBot="1"/>
+    <row r="12" spans="2:8" ht="51" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B12" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="129" t="str">
+        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],2,0)</f>
+        <v>Zdravstvena zaštita osoba starijih od 65 godina života, pod uslovom da nemaju zdravstveno osiguranje po drugom osnovu. Plaćanje neposrednog učešća u troškovima zdravstvene zaštite starijih od 65 godina života vršit će MRSRI KS, pod uslovom da nisu zdravstveno osigurani po drugom osnovu.</v>
+      </c>
+      <c r="F12" s="127" t="str">
+        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],6,0)</f>
+        <v xml:space="preserve">Općina, nadležna općinska služba
+Ministarstvo za rad, socijalnu politiku, raseljena lica i izbjeglice Kantona Sarajevo
+</v>
+      </c>
+      <c r="G12" s="127">
+        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="128">
+        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],9,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15" thickTop="1" thickBot="1">
+      <c r="B13" s="11"/>
+      <c r="E13" s="130"/>
+    </row>
+    <row r="14" spans="2:8" ht="51" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B14" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="E14" s="129" t="str">
+        <f>VLOOKUP(C14,Table5[],2,0)</f>
+        <v xml:space="preserve">Zaposlene osobe s invaliditetom imaju pravo na osnovni lični odbitak i umanjenje porezne osnovice po osnovu izdražavanja članova uže porodice i /ili po osnovu eventualne invalidnosti tih članova ili samog poreznog obveznika.
+Rezidentni porezni obveznici mogu odbiti i lični odbitak: 0,3 osnovnog ličnog odbitka iz stava (1) člana 24 za utvrđenu vlastitu invalidnost, kao i za utvrđenu invalidnost svakog člana uže porodice koje porezni obveznik izdržava. </v>
+      </c>
+      <c r="F14" s="127" t="str">
+        <f>VLOOKUP(C14,Table5[],6,0)</f>
+        <v>Poreska uprava nadležne općine</v>
+      </c>
+      <c r="G14" s="127">
+        <f>VLOOKUP(C14,Table5[],7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="128">
+        <f>VLOOKUP(C14,Table5[],9,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15" thickTop="1" thickBot="1">
+      <c r="B15" s="11"/>
+      <c r="E15" s="130"/>
+    </row>
+    <row r="16" spans="2:8" ht="51" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B16" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="129" t="str">
+        <f>VLOOKUP(C16,'Neinstitucionalizirana prava'!$A$2:$F$10,2,0)</f>
+        <v>Osoba može dobiti pomoć i njegu u kući ako ispunjava sljedeće uvjete:
+- Nije već dobila novčanu naknadu za pomoć i njegu od drugog.
+- Nema mogućnost da pomoć i njegu osiguraju roditelji, bračni partner ili djeca.
+- Nema mogućnost osiguranja pomoći i njege putem ugovora o doživotnom izdržavanju.
+- Prihod njezina kućanstva ne prelazi 30% prosječne plaće.</v>
+      </c>
+      <c r="F16" s="152" t="str">
+        <f>VLOOKUP(C16,'Neinstitucionalizirana prava'!$A$2:$F$10,4,0)</f>
+        <v>Zakon o socijalnoj zaštiti, zaštiti civilnih žrtava rata i zaštiti porodice sa djecom</v>
+      </c>
+      <c r="G16" s="152"/>
+      <c r="H16" s="153"/>
+    </row>
+    <row r="17" ht="14.4" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F16:H16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{36E09D36-0650-4C98-A3B4-174899F8F610}">
+          <x14:formula1>
+            <xm:f>Filter!$M$1:$M$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>C12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75DE1291-819C-4172-8F27-9C9DFC2BE22F}">
+          <x14:formula1>
+            <xm:f>Filter!$N$1:$N$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>C14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C16D060D-CB17-4A32-A1F1-CB0EAC63FF9A}">
+          <x14:formula1>
+            <xm:f>Filter!$O$1:$O$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>C16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B708E5-CA35-4FCC-AEE5-07D111DD3736}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:U18"/>
@@ -12067,16 +13370,16 @@
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="50.4" customHeight="1">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="160" t="s">
         <v>362</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="155"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -12096,127 +13399,134 @@
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="162" t="s">
+      <c r="C6" s="163" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="163"/>
+      <c r="D6" s="164"/>
     </row>
     <row r="7" spans="1:21" ht="31.5" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="164" t="s">
+      <c r="C7" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="164"/>
+      <c r="D7" s="165"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="B8" s="154" t="s">
+      <c r="B8" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="156" t="e">
+      <c r="C8" s="157" t="e">
         <f>VLOOKUP(C7,All,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D8" s="157"/>
+      <c r="D8" s="158"/>
     </row>
     <row r="9" spans="1:21" ht="78" customHeight="1">
-      <c r="B9" s="154"/>
-      <c r="C9" s="158"/>
-      <c r="D9" s="159"/>
+      <c r="B9" s="159"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="162"/>
     </row>
     <row r="10" spans="1:21" ht="28.5" customHeight="1">
       <c r="B10" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="C10" s="160" t="e">
+      <c r="C10" s="154" t="e">
         <f>VLOOKUP($C$7,Usluge,6,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D10" s="161"/>
+      <c r="D10" s="155"/>
     </row>
     <row r="11" spans="1:21" ht="15">
       <c r="B11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="160" t="e">
+      <c r="C11" s="154" t="e">
         <f>VLOOKUP($C$7,Usluge,7,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D11" s="161"/>
+      <c r="D11" s="155"/>
     </row>
     <row r="12" spans="1:21" ht="15">
       <c r="B12" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="160" t="e">
+      <c r="C12" s="154" t="e">
         <f>VLOOKUP($C$7,Usluge,8,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D12" s="161"/>
+      <c r="D12" s="155"/>
     </row>
     <row r="13" spans="1:21" ht="15">
       <c r="B13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="160" t="e">
+      <c r="C13" s="154" t="e">
         <f>VLOOKUP($C$7,Usluge,9,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D13" s="161"/>
+      <c r="D13" s="155"/>
     </row>
     <row r="14" spans="1:21" ht="15">
       <c r="B14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="160" t="e">
+      <c r="C14" s="154" t="e">
         <f>VLOOKUP($C$7,Usluge,10,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D14" s="161"/>
+      <c r="D14" s="155"/>
     </row>
     <row r="15" spans="1:21" ht="62.25" customHeight="1">
       <c r="B15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="156" t="e">
+      <c r="C15" s="157" t="e">
         <f>VLOOKUP($C$7,Usluge,11,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D15" s="157"/>
+      <c r="D15" s="158"/>
     </row>
     <row r="16" spans="1:21" ht="126" customHeight="1">
       <c r="B16" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="156" t="e">
+      <c r="C16" s="157" t="e">
         <f>VLOOKUP($C$7,Usluge,12,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D16" s="157"/>
+      <c r="D16" s="158"/>
     </row>
     <row r="17" spans="2:4" ht="15">
       <c r="B17" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="160" t="e">
+      <c r="C17" s="154" t="e">
         <f>VLOOKUP($C$7,Usluge,13,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D17" s="161"/>
+      <c r="D17" s="155"/>
     </row>
     <row r="18" spans="2:4" ht="15">
       <c r="B18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="165" t="e">
+      <c r="C18" s="156" t="e">
         <f>VLOOKUP($C$7,Usluge,15,0)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D18" s="165"/>
+      <c r="D18" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C12:D12"/>
@@ -12224,13 +13534,6 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12255,15 +13558,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79745D0-3A85-4CE4-80E0-563AD56B3BAC}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="134" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -12276,7 +13579,7 @@
     <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.9" customHeight="1">
+    <row r="1" spans="1:8" ht="24.9" customHeight="1">
       <c r="A1" s="108" t="s">
         <v>1</v>
       </c>
@@ -12295,8 +13598,14 @@
       <c r="F1" s="108" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="79.8">
+      <c r="G1" s="168" t="s">
+        <v>562</v>
+      </c>
+      <c r="H1" s="168" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="79.8">
       <c r="A2" s="110" t="s">
         <v>471</v>
       </c>
@@ -12313,8 +13622,16 @@
         <v>306</v>
       </c>
       <c r="F2" s="84"/>
-    </row>
-    <row r="3" spans="1:6" ht="182.4">
+      <c r="G2" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.833867749999897</v>
+      </c>
+      <c r="H2" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.3318392646853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="182.4">
       <c r="A3" s="110" t="s">
         <v>16</v>
       </c>
@@ -12333,8 +13650,16 @@
       <c r="F3" s="91" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="296.39999999999998">
+      <c r="G3" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.899231149999999</v>
+      </c>
+      <c r="H3" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.4151610950864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="296.39999999999998">
       <c r="A4" s="110" t="s">
         <v>539</v>
       </c>
@@ -12350,8 +13675,16 @@
       <c r="E4" s="110" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="171">
+      <c r="G4" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857481149999998</v>
+      </c>
+      <c r="H4" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.416157265859901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="171">
       <c r="A5" s="110" t="s">
         <v>57</v>
       </c>
@@ -12368,8 +13701,16 @@
         <v>308</v>
       </c>
       <c r="F5" s="110"/>
-    </row>
-    <row r="6" spans="1:6" ht="285">
+      <c r="G5" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.851796999999998</v>
+      </c>
+      <c r="H5" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.3827719453942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="285">
       <c r="A6" s="110" t="s">
         <v>48</v>
       </c>
@@ -12386,8 +13727,16 @@
         <v>252</v>
       </c>
       <c r="F6" s="84"/>
-    </row>
-    <row r="7" spans="1:6" ht="273.60000000000002">
+      <c r="G6" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857349450000001</v>
+      </c>
+      <c r="H6" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413135847170199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="273.60000000000002">
       <c r="A7" s="110" t="s">
         <v>58</v>
       </c>
@@ -12404,8 +13753,16 @@
         <v>310</v>
       </c>
       <c r="F7" s="84"/>
-    </row>
-    <row r="8" spans="1:6" ht="205.2">
+      <c r="G7" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857201400000001</v>
+      </c>
+      <c r="H7" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413743400000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="205.2">
       <c r="A8" s="110" t="s">
         <v>49</v>
       </c>
@@ -12422,8 +13779,16 @@
         <v>470</v>
       </c>
       <c r="F8" s="110"/>
-    </row>
-    <row r="9" spans="1:6" ht="102.6">
+      <c r="G8" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="H8" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="102.6">
       <c r="A9" s="110" t="s">
         <v>482</v>
       </c>
@@ -12440,8 +13805,16 @@
         <v>200</v>
       </c>
       <c r="F9" s="110"/>
-    </row>
-    <row r="10" spans="1:6" ht="102.6">
+      <c r="G9" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="H9" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="102.6">
       <c r="A10" s="111" t="s">
         <v>483</v>
       </c>
@@ -12458,10 +13831,18 @@
         <v>202</v>
       </c>
       <c r="F10" s="110"/>
+      <c r="G10" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="H10" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
-    <sortCondition ref="A6:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
+    <sortCondition ref="A6:A10"/>
   </sortState>
   <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="4" priority="1"/>
@@ -12476,15 +13857,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646CFECD-C102-4B70-A315-649D04135A21}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="O1" zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -12508,7 +13889,7 @@
     <col min="18" max="16384" width="9.109375" style="105"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="89" customFormat="1" ht="40.5" customHeight="1">
+    <row r="1" spans="1:19" s="89" customFormat="1" ht="40.5" customHeight="1">
       <c r="A1" s="85" t="s">
         <v>73</v>
       </c>
@@ -12560,8 +13941,14 @@
       <c r="Q1" s="85" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="93" customFormat="1" ht="124.2">
+      <c r="R1" s="168" t="s">
+        <v>562</v>
+      </c>
+      <c r="S1" s="168" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="93" customFormat="1" ht="124.2">
       <c r="A2" s="90">
         <v>1</v>
       </c>
@@ -12609,8 +13996,16 @@
         <v>369</v>
       </c>
       <c r="Q2" s="90"/>
-    </row>
-    <row r="3" spans="1:17" s="93" customFormat="1" ht="345">
+      <c r="R2" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.833867749999897</v>
+      </c>
+      <c r="S2" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.3318392646853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="93" customFormat="1" ht="345">
       <c r="A3" s="90">
         <v>3</v>
       </c>
@@ -12658,8 +14053,16 @@
       <c r="Q3" s="91" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" s="93" customFormat="1" ht="165.6">
+      <c r="R3" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.899231149999999</v>
+      </c>
+      <c r="S3" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.4151610950864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="93" customFormat="1" ht="165.6">
       <c r="A4" s="90">
         <v>4</v>
       </c>
@@ -12711,8 +14114,16 @@
       <c r="Q4" s="94" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" s="93" customFormat="1" ht="216" customHeight="1">
+      <c r="R4" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857481149999998</v>
+      </c>
+      <c r="S4" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.416157265859901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="93" customFormat="1" ht="216" customHeight="1">
       <c r="A5" s="90">
         <v>5</v>
       </c>
@@ -12760,8 +14171,16 @@
       <c r="Q5" s="90" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" s="93" customFormat="1" ht="179.4">
+      <c r="R5" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.851796999999998</v>
+      </c>
+      <c r="S5" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.3827719453942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="93" customFormat="1" ht="179.4">
       <c r="A6" s="90">
         <v>6</v>
       </c>
@@ -12809,8 +14228,16 @@
       <c r="Q6" s="90" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" s="93" customFormat="1" ht="132" customHeight="1">
+      <c r="R6" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857349450000001</v>
+      </c>
+      <c r="S6" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413135847170199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="93" customFormat="1" ht="132" customHeight="1">
       <c r="A7" s="90">
         <v>7</v>
       </c>
@@ -12862,8 +14289,16 @@
       <c r="Q7" s="99" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" s="93" customFormat="1" ht="86.4">
+      <c r="R7" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857201400000001</v>
+      </c>
+      <c r="S7" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413743400000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="93" customFormat="1" ht="86.4">
       <c r="A8" s="90">
         <v>8</v>
       </c>
@@ -12915,8 +14350,16 @@
       <c r="Q8" s="99" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" s="93" customFormat="1" ht="409.6">
+      <c r="R8" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="S8" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="93" customFormat="1" ht="409.6">
       <c r="A9" s="90">
         <v>9</v>
       </c>
@@ -12968,8 +14411,16 @@
       <c r="Q9" s="99" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" s="93" customFormat="1" ht="82.8">
+      <c r="R9" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="S9" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="93" customFormat="1" ht="82.8">
       <c r="A10" s="90">
         <v>10</v>
       </c>
@@ -13015,8 +14466,16 @@
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="90"/>
-    </row>
-    <row r="11" spans="1:17" s="93" customFormat="1" ht="124.2">
+      <c r="R10" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="S10" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="93" customFormat="1" ht="124.2">
       <c r="A11" s="90">
         <v>11</v>
       </c>
@@ -13068,8 +14527,16 @@
       <c r="Q11" s="99" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" s="93" customFormat="1" ht="220.8">
+      <c r="R11" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857349450000001</v>
+      </c>
+      <c r="S11" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413135847170199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="93" customFormat="1" ht="220.8">
       <c r="A12" s="90">
         <v>12</v>
       </c>
@@ -13119,8 +14586,16 @@
       <c r="Q12" s="90" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" s="93" customFormat="1" ht="55.2">
+      <c r="R12" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="S12" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="93" customFormat="1" ht="55.2">
       <c r="A13" s="90">
         <v>13</v>
       </c>
@@ -13166,8 +14641,16 @@
       </c>
       <c r="P13" s="92"/>
       <c r="Q13" s="90"/>
-    </row>
-    <row r="14" spans="1:17" s="93" customFormat="1" ht="82.8">
+      <c r="R13" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.84666275</v>
+      </c>
+      <c r="S13" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.354620012764201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="93" customFormat="1" ht="82.8">
       <c r="A14" s="90">
         <v>14</v>
       </c>
@@ -13213,8 +14696,16 @@
       </c>
       <c r="P14" s="92"/>
       <c r="Q14" s="90"/>
-    </row>
-    <row r="15" spans="1:17" s="93" customFormat="1" ht="234.6">
+      <c r="R14" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S14" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="93" customFormat="1" ht="234.6">
       <c r="A15" s="90">
         <v>15</v>
       </c>
@@ -13264,8 +14755,16 @@
         <v>60</v>
       </c>
       <c r="Q15" s="90"/>
-    </row>
-    <row r="16" spans="1:17" s="93" customFormat="1" ht="96" customHeight="1">
+      <c r="R15" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S15" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="93" customFormat="1" ht="96" customHeight="1">
       <c r="A16" s="90">
         <v>16</v>
       </c>
@@ -13315,8 +14814,16 @@
         <v>60</v>
       </c>
       <c r="Q16" s="90"/>
-    </row>
-    <row r="17" spans="1:17" s="93" customFormat="1" ht="151.80000000000001">
+      <c r="R16" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S16" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" s="93" customFormat="1" ht="151.80000000000001">
       <c r="A17" s="90">
         <v>17</v>
       </c>
@@ -13366,8 +14873,16 @@
         <v>60</v>
       </c>
       <c r="Q17" s="90"/>
-    </row>
-    <row r="18" spans="1:17" s="93" customFormat="1" ht="303.60000000000002">
+      <c r="R17" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S17" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="93" customFormat="1" ht="303.60000000000002">
       <c r="A18" s="90">
         <v>18</v>
       </c>
@@ -13417,8 +14932,16 @@
       <c r="Q18" s="90" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" s="93" customFormat="1" ht="179.4">
+      <c r="R18" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S18" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="93" customFormat="1" ht="179.4">
       <c r="A19" s="90">
         <v>19</v>
       </c>
@@ -13468,8 +14991,16 @@
         <v>60</v>
       </c>
       <c r="Q19" s="90"/>
-    </row>
-    <row r="20" spans="1:17" s="93" customFormat="1" ht="55.2">
+      <c r="R19" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85358815</v>
+      </c>
+      <c r="S19" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.394800338932299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="93" customFormat="1" ht="55.2">
       <c r="A20" s="90">
         <v>20</v>
       </c>
@@ -13519,8 +15050,16 @@
         <v>60</v>
       </c>
       <c r="Q20" s="90"/>
-    </row>
-    <row r="21" spans="1:17" s="93" customFormat="1" ht="234.6">
+      <c r="R20" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S20" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="93" customFormat="1" ht="234.6">
       <c r="A21" s="90">
         <v>21</v>
       </c>
@@ -13568,8 +15107,16 @@
       </c>
       <c r="P21" s="92"/>
       <c r="Q21" s="90"/>
-    </row>
-    <row r="22" spans="1:17" s="103" customFormat="1" ht="219.75" customHeight="1">
+      <c r="R21" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S21" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="103" customFormat="1" ht="219.75" customHeight="1">
       <c r="A22" s="90">
         <v>22</v>
       </c>
@@ -13621,8 +15168,16 @@
       <c r="Q22" s="99" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" s="93" customFormat="1" ht="262.2">
+      <c r="R22" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.843953499999998</v>
+      </c>
+      <c r="S22" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="93" customFormat="1" ht="262.2">
       <c r="A23" s="90">
         <v>23</v>
       </c>
@@ -13668,8 +15223,16 @@
       <c r="Q23" s="90" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" s="93" customFormat="1" ht="55.2">
+      <c r="R23" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="S23" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="93" customFormat="1" ht="55.2">
       <c r="A24" s="90">
         <v>24</v>
       </c>
@@ -13721,8 +15284,16 @@
       <c r="Q24" s="99" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" s="93" customFormat="1" ht="138">
+      <c r="R24" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.833867749999897</v>
+      </c>
+      <c r="S24" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.3318392646853</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" s="93" customFormat="1" ht="138">
       <c r="A25" s="90">
         <v>25</v>
       </c>
@@ -13766,8 +15337,16 @@
       <c r="O25" s="90"/>
       <c r="P25" s="92"/>
       <c r="Q25" s="90"/>
-    </row>
-    <row r="26" spans="1:17" s="93" customFormat="1" ht="220.8">
+      <c r="R25" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.85633</v>
+      </c>
+      <c r="S25" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" s="93" customFormat="1" ht="220.8">
       <c r="A26" s="90">
         <v>26</v>
       </c>
@@ -13813,8 +15392,16 @@
       <c r="Q26" s="90" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" s="93" customFormat="1" ht="409.6">
+      <c r="R26" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.856848849999999</v>
+      </c>
+      <c r="S26" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.384989102369499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="93" customFormat="1" ht="409.6">
       <c r="A27" s="90">
         <v>27</v>
       </c>
@@ -13862,8 +15449,16 @@
       <c r="Q27" s="90" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" s="93" customFormat="1" ht="409.6">
+      <c r="R27" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.833867749999897</v>
+      </c>
+      <c r="S27" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.3318392646853</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="93" customFormat="1" ht="409.6">
       <c r="A28" s="90">
         <v>28</v>
       </c>
@@ -13911,8 +15506,16 @@
       <c r="Q28" s="90" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" s="93" customFormat="1" ht="409.6">
+      <c r="R28" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857201400000001</v>
+      </c>
+      <c r="S28" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413743400000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="93" customFormat="1" ht="409.6">
       <c r="A29" s="90">
         <v>29</v>
       </c>
@@ -13954,8 +15557,16 @@
       </c>
       <c r="P29" s="92"/>
       <c r="Q29" s="90"/>
-    </row>
-    <row r="30" spans="1:17" s="93" customFormat="1" ht="179.4">
+      <c r="R29" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>43.857201400000001</v>
+      </c>
+      <c r="S29" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>18.413743400000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="93" customFormat="1" ht="179.4">
       <c r="A30" s="90">
         <v>30</v>
       </c>
@@ -13997,8 +15608,16 @@
       <c r="Q30" s="90" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" s="135" customFormat="1" ht="345.6">
+      <c r="R30" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" s="135" customFormat="1" ht="345.6">
       <c r="A31" s="99">
         <v>31</v>
       </c>
@@ -14042,8 +15661,16 @@
       </c>
       <c r="P31" s="92"/>
       <c r="Q31" s="90"/>
-    </row>
-    <row r="32" spans="1:17" s="135" customFormat="1" ht="248.4">
+      <c r="R31" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="93">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="135" customFormat="1" ht="248.4">
       <c r="A32" s="104">
         <v>31</v>
       </c>
@@ -14087,8 +15714,16 @@
       </c>
       <c r="P32" s="137"/>
       <c r="Q32" s="136"/>
-    </row>
-    <row r="33" spans="1:17" s="135" customFormat="1" ht="409.6">
+      <c r="R32" s="169">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="170">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="135" customFormat="1" ht="409.6">
       <c r="A33" s="104">
         <v>31</v>
       </c>
@@ -14132,6 +15767,14 @@
       </c>
       <c r="P33" s="137"/>
       <c r="Q33" s="136"/>
+      <c r="R33" s="169">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,2,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S33" s="170">
+        <f>IFERROR(VLOOKUP([1]!Table2[[#This Row],[Adresa]],[1]Sheet1!$A$1:$C$20,3,0),0)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q30">
@@ -14253,7 +15896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EE97C4-5CE4-4386-BABA-CA4D0DFA0DEA}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:Q28"/>
@@ -15116,7 +16759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AECC7D0-5F0E-45C9-9C31-E98820A856AD}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:Q64"/>
@@ -17971,7 +19614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4A8391-2707-49BC-A199-F020DD08ECF4}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I44"/>
@@ -27591,6 +29234,244 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E157FB-72B3-4C4B-85B7-17A5CFA382E2}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="166" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2">
+        <v>43.858553000000001</v>
+      </c>
+      <c r="C2">
+        <v>18.402099609375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="166" t="s">
+        <v>295</v>
+      </c>
+      <c r="B3">
+        <v>43.857349450000001</v>
+      </c>
+      <c r="C3">
+        <v>18.413135847170199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="166" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4">
+        <v>43.829455600000003</v>
+      </c>
+      <c r="C4">
+        <v>18.310951865680199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="166" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5">
+        <v>43.847950949999998</v>
+      </c>
+      <c r="C5">
+        <v>18.3536972495775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="166" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6">
+        <v>43.852587649999997</v>
+      </c>
+      <c r="C6">
+        <v>18.3816443990954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="167" t="s">
+        <v>421</v>
+      </c>
+      <c r="B7">
+        <v>43.85633</v>
+      </c>
+      <c r="C7">
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="166" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8">
+        <v>43.857349450000001</v>
+      </c>
+      <c r="C8">
+        <v>18.413135847170199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="166" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9">
+        <v>43.8671705</v>
+      </c>
+      <c r="C9">
+        <v>18.413270799999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10">
+        <v>43.833867749999897</v>
+      </c>
+      <c r="C10">
+        <v>18.3318392646853</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>43.899231149999999</v>
+      </c>
+      <c r="C11">
+        <v>18.4151610950864</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12">
+        <v>43.857481149999998</v>
+      </c>
+      <c r="C12">
+        <v>18.416157265859901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13">
+        <v>43.851796999999998</v>
+      </c>
+      <c r="C13">
+        <v>18.3827719453942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14">
+        <v>43.857349450000001</v>
+      </c>
+      <c r="C14">
+        <v>18.413135847170199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B15">
+        <v>43.857201400000001</v>
+      </c>
+      <c r="C15">
+        <v>18.413743400000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16">
+        <v>43.85633</v>
+      </c>
+      <c r="C16">
+        <v>18.384492399999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17">
+        <v>43.84666275</v>
+      </c>
+      <c r="C17">
+        <v>18.354620012764201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18">
+        <v>43.843953499999998</v>
+      </c>
+      <c r="C18">
+        <v>18.358142300000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19">
+        <v>43.85358815</v>
+      </c>
+      <c r="C19">
+        <v>18.394800338932299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20">
+        <v>43.856848849999999</v>
+      </c>
+      <c r="C20">
+        <v>18.384989102369499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B08CEF-B1A5-4F52-AFAF-57F34C0EBCF1}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
@@ -27604,7 +29485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002E9750-F5D3-4D85-9C68-E88E476AEE21}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B1:U28"/>
@@ -27753,7 +29634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C51CCA2-5B7B-4350-BE22-34019BA8ED20}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:H17"/>
@@ -27892,7 +29773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E983FD8-F479-4424-8A37-22417D59F505}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:H17"/>
@@ -28081,7 +29962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D7C7FC-29AF-4F20-9BCD-2B72AB52BFA5}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B2:H17"/>
@@ -28221,149 +30102,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6717636-9D63-4CEF-B4BB-541077ED8170}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="B2:H17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="13.8"/>
-  <cols>
-    <col min="1" max="1" width="8.5546875" style="10"/>
-    <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="76" style="15" customWidth="1"/>
-    <col min="4" max="4" width="3.5546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="77.5546875" style="125" customWidth="1"/>
-    <col min="6" max="8" width="14.88671875" style="125" customWidth="1"/>
-    <col min="9" max="16384" width="8.5546875" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" ht="14.4">
-      <c r="B2"/>
-    </row>
-    <row r="3" spans="2:8" ht="14.4">
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="2:8" ht="14.4">
-      <c r="B4"/>
-    </row>
-    <row r="11" spans="2:8" ht="14.4" thickBot="1"/>
-    <row r="12" spans="2:8" ht="51" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B12" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="129" t="str">
-        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],2,0)</f>
-        <v>Zdravstvena zaštita osoba starijih od 65 godina života, pod uslovom da nemaju zdravstveno osiguranje po drugom osnovu. Plaćanje neposrednog učešća u troškovima zdravstvene zaštite starijih od 65 godina života vršit će MRSRI KS, pod uslovom da nisu zdravstveno osigurani po drugom osnovu.</v>
-      </c>
-      <c r="F12" s="127" t="str">
-        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],6,0)</f>
-        <v xml:space="preserve">Općina, nadležna općinska služba
-Ministarstvo za rad, socijalnu politiku, raseljena lica i izbjeglice Kantona Sarajevo
-</v>
-      </c>
-      <c r="G12" s="127">
-        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="128">
-        <f>VLOOKUP(C12,Table2[[Naziv ]:[Dodatne napomene]],9,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="15" thickTop="1" thickBot="1">
-      <c r="B13" s="11"/>
-      <c r="E13" s="130"/>
-    </row>
-    <row r="14" spans="2:8" ht="51" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="E14" s="129" t="str">
-        <f>VLOOKUP(C14,Table5[],2,0)</f>
-        <v xml:space="preserve">Zaposlene osobe s invaliditetom imaju pravo na osnovni lični odbitak i umanjenje porezne osnovice po osnovu izdražavanja članova uže porodice i /ili po osnovu eventualne invalidnosti tih članova ili samog poreznog obveznika.
-Rezidentni porezni obveznici mogu odbiti i lični odbitak: 0,3 osnovnog ličnog odbitka iz stava (1) člana 24 za utvrđenu vlastitu invalidnost, kao i za utvrđenu invalidnost svakog člana uže porodice koje porezni obveznik izdržava. </v>
-      </c>
-      <c r="F14" s="127" t="str">
-        <f>VLOOKUP(C14,Table5[],6,0)</f>
-        <v>Poreska uprava nadležne općine</v>
-      </c>
-      <c r="G14" s="127">
-        <f>VLOOKUP(C14,Table5[],7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="128">
-        <f>VLOOKUP(C14,Table5[],9,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="15" thickTop="1" thickBot="1">
-      <c r="B15" s="11"/>
-      <c r="E15" s="130"/>
-    </row>
-    <row r="16" spans="2:8" ht="51" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B16" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="129" t="str">
-        <f>VLOOKUP(C16,'Neinstitucionalizirana prava'!$A$2:$F$10,2,0)</f>
-        <v>Osoba može dobiti pomoć i njegu u kući ako ispunjava sljedeće uvjete:
-- Nije već dobila novčanu naknadu za pomoć i njegu od drugog.
-- Nema mogućnost da pomoć i njegu osiguraju roditelji, bračni partner ili djeca.
-- Nema mogućnost osiguranja pomoći i njege putem ugovora o doživotnom izdržavanju.
-- Prihod njezina kućanstva ne prelazi 30% prosječne plaće.</v>
-      </c>
-      <c r="F16" s="152" t="str">
-        <f>VLOOKUP(C16,'Neinstitucionalizirana prava'!$A$2:$F$10,4,0)</f>
-        <v>Zakon o socijalnoj zaštiti, zaštiti civilnih žrtava rata i zaštiti porodice sa djecom</v>
-      </c>
-      <c r="G16" s="152"/>
-      <c r="H16" s="153"/>
-    </row>
-    <row r="17" ht="14.4" thickTop="1"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F16:H16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{36E09D36-0650-4C98-A3B4-174899F8F610}">
-          <x14:formula1>
-            <xm:f>Filter!$M$1:$M$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>C12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75DE1291-819C-4172-8F27-9C9DFC2BE22F}">
-          <x14:formula1>
-            <xm:f>Filter!$N$1:$N$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>C14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C16D060D-CB17-4A32-A1F1-CB0EAC63FF9A}">
-          <x14:formula1>
-            <xm:f>Filter!$O$1:$O$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>C16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>